<commit_message>
Update of the results : increasing the convergence required leads to better picture and slightly better Z parameters vs ANITITER II
</commit_message>
<xml_diff>
--- a/Test Configurations/ICRH/ICRH_HFSS_Results.xlsx
+++ b/Test Configurations/ICRH/ICRH_HFSS_Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="324" windowWidth="21828" windowHeight="9000"/>
+    <workbookView xWindow="768" yWindow="324" windowWidth="19392" windowHeight="8712"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
   <si>
     <t>e_strap [mm]</t>
   </si>
@@ -192,63 +192,15 @@
     <t>Constant density</t>
   </si>
   <si>
-    <t>Z11 [Ohm]</t>
-  </si>
-  <si>
-    <t>Z21 [Ohm]</t>
-  </si>
-  <si>
-    <t>0.238+23.862i</t>
-  </si>
-  <si>
-    <t>0.236+4.320i</t>
-  </si>
-  <si>
-    <t>0.993+24.530i</t>
-  </si>
-  <si>
-    <t>0.9158+4.578i</t>
-  </si>
-  <si>
-    <t>2.065+24.712i</t>
-  </si>
-  <si>
-    <t>1.703+4.408i</t>
-  </si>
-  <si>
     <t>HFSS</t>
   </si>
   <si>
-    <t>0.218 + i23.31</t>
-  </si>
-  <si>
-    <t>1.68 + i23.52</t>
-  </si>
-  <si>
-    <t>0.215 + i3.42</t>
-  </si>
-  <si>
-    <t>1.53 + i3.49</t>
-  </si>
-  <si>
     <t>ANTITER</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>1.212+24.613i</t>
-  </si>
-  <si>
-    <t>1.093+4.589i</t>
-  </si>
-  <si>
-    <t>1.167 + 24.585i</t>
-  </si>
-  <si>
-    <t>1.061 + 4.105i</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -271,13 +223,85 @@
   </si>
   <si>
     <t>Equivalent Dielectric Permittivity</t>
+  </si>
+  <si>
+    <t>1e15 to 5e18</t>
+  </si>
+  <si>
+    <t>Re Z11</t>
+  </si>
+  <si>
+    <t>Im Z11</t>
+  </si>
+  <si>
+    <t>Re Z21</t>
+  </si>
+  <si>
+    <t>Im Z21</t>
+  </si>
+  <si>
+    <t>Re Z11 [Ohm]</t>
+  </si>
+  <si>
+    <t>Re Z21 [Ohm]</t>
+  </si>
+  <si>
+    <t>1 to 132.72</t>
+  </si>
+  <si>
+    <t>1 to 66.86</t>
+  </si>
+  <si>
+    <t>Im Z21 [Ohm]</t>
+  </si>
+  <si>
+    <t>Relative difference vs ANTITER in %</t>
+  </si>
+  <si>
+    <t>Inhomo. plasma and own PML</t>
+  </si>
+  <si>
+    <t>1e15 to 10e18</t>
+  </si>
+  <si>
+    <t>Inhomo. dielectric and own PML</t>
+  </si>
+  <si>
+    <t>Inhomo. dielectric and radiation BC</t>
+  </si>
+  <si>
+    <t>0.98 to -78.6</t>
+  </si>
+  <si>
+    <t>0 to 144.7</t>
+  </si>
+  <si>
+    <t>"-31 to -161278"</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>0.98 to -158</t>
+  </si>
+  <si>
+    <t>0 to 964</t>
+  </si>
+  <si>
+    <t>"-31 to -322557"</t>
+  </si>
+  <si>
+    <t>Solved elements for dS=1e-3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,8 +464,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -642,6 +673,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -806,7 +843,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -814,33 +851,18 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -854,6 +876,30 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -917,6 +963,141 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="107"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="7"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1e15 to 5e18</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>(Summary!$H$9,Summary!$P$9,Summary!$I$9,Summary!$Q$9,Summary!$J$9,Summary!$R$9,Summary!$K$9,Summary!$S$9,Summary!$L$9,Summary!$T$9)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.6000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.724</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.314</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0519999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="192350464"/>
+        <c:axId val="192368640"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="192350464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="192368640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="192368640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="192350464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
@@ -925,7 +1106,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1070,11 +1250,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="193075072"/>
-        <c:axId val="193076608"/>
+        <c:axId val="193298816"/>
+        <c:axId val="193300352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="193075072"/>
+        <c:axId val="193298816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1084,12 +1264,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193076608"/>
+        <c:crossAx val="193300352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="193076608"/>
+        <c:axId val="193300352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1100,14 +1280,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193075072"/>
+        <c:crossAx val="193298816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1123,6 +1302,41 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1444,10 +1658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1457,120 +1671,209 @@
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
     <col min="6" max="6" width="7.88671875" customWidth="1"/>
-    <col min="7" max="7" width="2.44140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="1.33203125" style="5" customWidth="1"/>
     <col min="8" max="8" width="7.5546875" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="2" style="18" customWidth="1"/>
-    <col min="13" max="13" width="6.77734375" customWidth="1"/>
-    <col min="14" max="14" width="14.21875" customWidth="1"/>
-    <col min="15" max="15" width="13.21875" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" customWidth="1"/>
+    <col min="12" max="12" width="7.21875" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" customWidth="1"/>
+    <col min="15" max="15" width="1.109375" style="13" customWidth="1"/>
+    <col min="16" max="16" width="6.77734375" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" customWidth="1"/>
+    <col min="18" max="18" width="7.77734375" customWidth="1"/>
+    <col min="19" max="19" width="5.33203125" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" customWidth="1"/>
+    <col min="21" max="21" width="1" style="5" customWidth="1"/>
+    <col min="22" max="22" width="13.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C1" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="H1" s="7" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="C1" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="H1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="V1" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+    </row>
+    <row r="2" spans="1:26" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="8" t="s">
+      <c r="O2" s="11"/>
+      <c r="P2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-    </row>
-    <row r="2" spans="1:15" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="S2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="T2" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="U2" s="9"/>
+      <c r="V2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="6">
         <v>81</v>
       </c>
-      <c r="B3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3">
-        <v>81</v>
-      </c>
-      <c r="H3" s="9">
+      <c r="H3" s="6">
         <v>0.51</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="9">
+      <c r="I3" s="6">
+        <v>1.212</v>
+      </c>
+      <c r="J3" s="6">
+        <v>24.61</v>
+      </c>
+      <c r="K3" s="6">
+        <v>1.093</v>
+      </c>
+      <c r="L3" s="6">
+        <v>4.5890000000000004</v>
+      </c>
+      <c r="M3" s="6">
+        <v>63842</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="O3" s="12"/>
+      <c r="P3" s="6">
         <v>0.53</v>
       </c>
-      <c r="N3" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="Q3" s="6">
+        <v>1.167</v>
+      </c>
+      <c r="R3" s="6">
+        <v>24.59</v>
+      </c>
+      <c r="S3" s="6">
+        <v>1.0609999999999999</v>
+      </c>
+      <c r="T3" s="6">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="V3" s="17">
+        <f>ABS(H3-P3)/P3*100</f>
+        <v>3.7735849056603805</v>
+      </c>
+      <c r="W3" s="17">
+        <f t="shared" ref="W3:Z15" si="0">ABS(I3-Q3)/Q3*100</f>
+        <v>3.8560411311053922</v>
+      </c>
+      <c r="X3" s="17">
+        <f t="shared" si="0"/>
+        <v>8.1333875559168656E-2</v>
+      </c>
+      <c r="Y3" s="17">
+        <f t="shared" si="0"/>
+        <v>3.0160226201696538</v>
+      </c>
+      <c r="Z3" s="17">
+        <f t="shared" si="0"/>
+        <v>11.654501216545013</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
         <v>57</v>
       </c>
       <c r="B4">
@@ -1585,32 +1888,65 @@
       <c r="E4">
         <v>-32255</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="6">
         <v>14.17</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="9">
+      <c r="I4" s="6">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="J4" s="6">
+        <v>23.86</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="L4" s="6">
+        <v>4.32</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="6">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="N4" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
+      <c r="Q4" s="6">
+        <v>0.218</v>
+      </c>
+      <c r="R4" s="6">
+        <v>23.31</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0.215</v>
+      </c>
+      <c r="T4" s="6">
+        <v>3.42</v>
+      </c>
+      <c r="V4" s="17">
+        <f t="shared" ref="V4:V15" si="1">ABS(H4-P4)/P4*100</f>
+        <v>58.82352941176471</v>
+      </c>
+      <c r="W4" s="17">
+        <f t="shared" si="0"/>
+        <v>9.1743119266054993</v>
+      </c>
+      <c r="X4" s="17">
+        <f t="shared" si="0"/>
+        <v>2.3595023595023625</v>
+      </c>
+      <c r="Y4" s="17">
+        <f t="shared" si="0"/>
+        <v>9.7674418604651123</v>
+      </c>
+      <c r="Z4" s="17">
+        <f t="shared" si="0"/>
+        <v>26.31578947368422</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A5" s="18"/>
       <c r="B5">
         <v>5</v>
       </c>
@@ -1623,32 +1959,65 @@
       <c r="E5">
         <v>-161277</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="6">
         <v>66.86</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="6">
         <v>0.34399999999999997</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="9">
+      <c r="I5" s="6">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="J5" s="6">
+        <v>24.53</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0.91579999999999995</v>
+      </c>
+      <c r="L5" s="6">
+        <v>4.58</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="6">
         <v>0.74</v>
       </c>
-      <c r="N5" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
+      <c r="Q5" s="6">
+        <v>1.68</v>
+      </c>
+      <c r="R5" s="6">
+        <v>23.52</v>
+      </c>
+      <c r="S5" s="6">
+        <v>1.53</v>
+      </c>
+      <c r="T5" s="6">
+        <v>3.49</v>
+      </c>
+      <c r="V5" s="17">
+        <f t="shared" si="1"/>
+        <v>53.513513513513523</v>
+      </c>
+      <c r="W5" s="17">
+        <f t="shared" si="0"/>
+        <v>40.892857142857139</v>
+      </c>
+      <c r="X5" s="17">
+        <f t="shared" si="0"/>
+        <v>4.2942176870748368</v>
+      </c>
+      <c r="Y5" s="17">
+        <f t="shared" si="0"/>
+        <v>40.143790849673202</v>
+      </c>
+      <c r="Z5" s="17">
+        <f t="shared" si="0"/>
+        <v>31.232091690544404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
       <c r="B6">
         <v>10</v>
       </c>
@@ -1661,40 +2030,524 @@
       <c r="E6">
         <v>-322557</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>132.72</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="6">
         <v>1.6</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="9">
+      <c r="I6" s="6">
+        <v>2.0649999999999999</v>
+      </c>
+      <c r="J6" s="6">
+        <v>24.71</v>
+      </c>
+      <c r="K6" s="6">
+        <v>1.7030000000000001</v>
+      </c>
+      <c r="L6" s="6">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M6" s="6"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="6">
         <v>3.5</v>
       </c>
-      <c r="N6" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>40</v>
+      <c r="Q6" s="6">
+        <v>2.62</v>
+      </c>
+      <c r="R6" s="6">
+        <v>22.39</v>
+      </c>
+      <c r="S6" s="6">
+        <v>1.92</v>
+      </c>
+      <c r="T6" s="6">
+        <v>2.08</v>
+      </c>
+      <c r="V6" s="17">
+        <f t="shared" si="1"/>
+        <v>54.285714285714285</v>
+      </c>
+      <c r="W6" s="17">
+        <f t="shared" si="0"/>
+        <v>21.183206106870234</v>
+      </c>
+      <c r="X6" s="17">
+        <f t="shared" si="0"/>
+        <v>10.361768646717286</v>
+      </c>
+      <c r="Y6" s="17">
+        <f t="shared" si="0"/>
+        <v>11.302083333333327</v>
+      </c>
+      <c r="Z6" s="17">
+        <f t="shared" si="0"/>
+        <v>111.53846153846155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" s="13" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="12"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17"/>
+    </row>
+    <row r="8" spans="1:26" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="J8" s="6">
+        <v>23.8</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.496</v>
+      </c>
+      <c r="L8" s="6">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="M8" s="6">
+        <v>18619</v>
+      </c>
+      <c r="P8" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R8" s="6">
+        <v>23.01</v>
+      </c>
+      <c r="S8" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="T8" s="6">
+        <v>3.12</v>
+      </c>
+      <c r="V8" s="17">
+        <f t="shared" si="1"/>
+        <v>7.9999999999999964</v>
+      </c>
+      <c r="W8" s="17">
+        <f t="shared" si="0"/>
+        <v>6.6000000000000059</v>
+      </c>
+      <c r="X8" s="17">
+        <f t="shared" si="0"/>
+        <v>3.4332898739678361</v>
+      </c>
+      <c r="Y8" s="17">
+        <f t="shared" si="0"/>
+        <v>10.222222222222218</v>
+      </c>
+      <c r="Z8" s="17">
+        <f t="shared" si="0"/>
+        <v>31.730769230769234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
+      <c r="B9" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="6">
+        <v>9.4E-2</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="J9" s="6">
+        <v>23.724</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.314</v>
+      </c>
+      <c r="L9" s="6">
+        <v>4.0519999999999996</v>
+      </c>
+      <c r="M9" s="6">
+        <v>23425</v>
+      </c>
+      <c r="P9" s="6">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="R9" s="6">
+        <v>23.13</v>
+      </c>
+      <c r="S9" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="T9" s="6">
+        <v>3.22</v>
+      </c>
+      <c r="V9" s="17">
+        <f t="shared" si="1"/>
+        <v>2.0833333333333353</v>
+      </c>
+      <c r="W9" s="17">
+        <f t="shared" si="0"/>
+        <v>3.4375000000000031</v>
+      </c>
+      <c r="X9" s="17">
+        <f t="shared" si="0"/>
+        <v>2.5680933852140129</v>
+      </c>
+      <c r="Y9" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2903225806451626</v>
+      </c>
+      <c r="Z9" s="17">
+        <f t="shared" si="0"/>
+        <v>25.838509316770164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="13" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="12"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
+    </row>
+    <row r="11" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.498</v>
+      </c>
+      <c r="J11" s="6">
+        <v>23.69</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.46</v>
+      </c>
+      <c r="L11" s="6">
+        <v>4.05</v>
+      </c>
+      <c r="M11" s="6">
+        <v>75720</v>
+      </c>
+      <c r="P11" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R11" s="6">
+        <v>23.01</v>
+      </c>
+      <c r="S11" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="T11" s="6">
+        <v>3.12</v>
+      </c>
+      <c r="V11" s="17">
+        <f t="shared" si="1"/>
+        <v>7.9999999999999964</v>
+      </c>
+      <c r="W11" s="17">
+        <f t="shared" si="0"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="X11" s="17">
+        <f t="shared" si="0"/>
+        <v>2.9552368535419369</v>
+      </c>
+      <c r="Y11" s="17">
+        <f t="shared" si="0"/>
+        <v>2.2222222222222241</v>
+      </c>
+      <c r="Z11" s="17">
+        <f t="shared" si="0"/>
+        <v>29.807692307692296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="6">
+        <v>9.4E-2</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="J12" s="6">
+        <v>23.5</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L12" s="6">
+        <v>3.96</v>
+      </c>
+      <c r="M12" s="6">
+        <v>21680</v>
+      </c>
+      <c r="P12" s="6">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="R12" s="6">
+        <v>23.13</v>
+      </c>
+      <c r="S12" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="T12" s="6">
+        <v>3.22</v>
+      </c>
+      <c r="V12" s="17">
+        <f t="shared" si="1"/>
+        <v>2.0833333333333353</v>
+      </c>
+      <c r="W12" s="17">
+        <f t="shared" si="0"/>
+        <v>3.1250000000000027</v>
+      </c>
+      <c r="X12" s="17">
+        <f t="shared" si="0"/>
+        <v>1.5996541288370125</v>
+      </c>
+      <c r="Y12" s="17">
+        <f t="shared" si="0"/>
+        <v>6.4516129032258114</v>
+      </c>
+      <c r="Z12" s="17">
+        <f t="shared" si="0"/>
+        <v>22.981366459627321</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="13" customFormat="1" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="12"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+    </row>
+    <row r="14" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.65</v>
+      </c>
+      <c r="J14" s="6">
+        <v>23.3</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="L14" s="6">
+        <v>3.74</v>
+      </c>
+      <c r="M14" s="6">
+        <v>187100</v>
+      </c>
+      <c r="N14" s="7"/>
+      <c r="P14" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R14" s="6">
+        <v>23.01</v>
+      </c>
+      <c r="S14" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="T14" s="6">
+        <v>3.12</v>
+      </c>
+      <c r="V14" s="17">
+        <f t="shared" si="1"/>
+        <v>19.999999999999996</v>
+      </c>
+      <c r="W14" s="17">
+        <f t="shared" si="0"/>
+        <v>30.000000000000004</v>
+      </c>
+      <c r="X14" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2603215993046464</v>
+      </c>
+      <c r="Y14" s="17">
+        <f t="shared" si="0"/>
+        <v>25.999999999999986</v>
+      </c>
+      <c r="Z14" s="17">
+        <f t="shared" si="0"/>
+        <v>19.871794871794872</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18"/>
+      <c r="B15" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0.11</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="J15" s="6">
+        <v>23.26</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0.37</v>
+      </c>
+      <c r="L15" s="6">
+        <v>3.84</v>
+      </c>
+      <c r="M15" s="6">
+        <v>285413</v>
+      </c>
+      <c r="N15" s="6"/>
+      <c r="P15" s="6">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="R15" s="6">
+        <v>23.13</v>
+      </c>
+      <c r="S15" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="T15" s="6">
+        <v>3.22</v>
+      </c>
+      <c r="V15" s="17">
+        <f t="shared" si="1"/>
+        <v>14.583333333333332</v>
+      </c>
+      <c r="W15" s="17">
+        <f t="shared" si="0"/>
+        <v>23.437500000000004</v>
+      </c>
+      <c r="X15" s="17">
+        <f t="shared" si="0"/>
+        <v>0.56204063986166264</v>
+      </c>
+      <c r="Y15" s="17">
+        <f t="shared" si="0"/>
+        <v>19.35483870967742</v>
+      </c>
+      <c r="Z15" s="17">
+        <f t="shared" si="0"/>
+        <v>19.254658385093158</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="H1:N1"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:T1"/>
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="K3:K6"/>
+    <mergeCell ref="N3:N6"/>
   </mergeCells>
+  <conditionalFormatting sqref="V1:Z1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>